<commit_message>
ASVS  2.2.3(Send email to user)
</commit_message>
<xml_diff>
--- a/analysis/checklist_app_sec.xlsx
+++ b/analysis/checklist_app_sec.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Architecture" sheetId="1" state="visible" r:id="rId3"/>
@@ -4019,13 +4019,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="30417430"/>
-        <c:axId val="60947789"/>
+        <c:axId val="51102087"/>
+        <c:axId val="10914346"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="30417430"/>
+        <c:axId val="51102087"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4063,7 +4063,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60947789"/>
+        <c:crossAx val="10914346"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4071,7 +4071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60947789"/>
+        <c:axId val="10914346"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4114,7 +4114,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30417430"/>
+        <c:crossAx val="51102087"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4178,9 +4178,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>15120</xdr:colOff>
+      <xdr:colOff>14760</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>36360</xdr:rowOff>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4189,7 +4189,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13680" y="4572720"/>
-        <a:ext cx="10967400" cy="9331920"/>
+        <a:ext cx="10967040" cy="9331560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4315,7 +4315,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C42" activeCellId="0" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -6352,7 +6352,7 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -6615,7 +6615,7 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -6918,8 +6918,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7127,7 +7127,7 @@
       <c r="I8" s="17"/>
       <c r="J8" s="21"/>
     </row>
-    <row r="9" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="44"/>
       <c r="B9" s="106" t="s">
         <v>615</v>
@@ -7142,7 +7142,7 @@
       <c r="F9" s="83" t="s">
         <v>616</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="24" t="s">
         <v>13</v>
       </c>
       <c r="H9" s="24"/>
@@ -7176,7 +7176,7 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -7597,7 +7597,7 @@
   </sheetPr>
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -8021,7 +8021,7 @@
   </sheetPr>
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -8679,7 +8679,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -10019,8 +10019,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12554,7 +12554,7 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -13192,7 +13192,7 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -13510,7 +13510,7 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -14264,8 +14264,8 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14705,7 +14705,7 @@
   </sheetPr>
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -15083,7 +15083,7 @@
   </sheetPr>
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ASVS 3.3.2, send email on password change, authentication revised
</commit_message>
<xml_diff>
--- a/analysis/checklist_app_sec.xlsx
+++ b/analysis/checklist_app_sec.xlsx
@@ -939,7 +939,7 @@
     <t xml:space="preserve">Verify the application only stores session tokens in the browser using secure methods such as appropriately secured cookies (see section 3.4) or HTML 5 session storage.</t>
   </si>
   <si>
-    <t xml:space="preserve">Can be implemented with Flask’s built-in session management capabilities</t>
+    <t xml:space="preserve">Can be implemented with Flask’s built-in session management capabilities, also solves 3.4 section</t>
   </si>
   <si>
     <t xml:space="preserve">3.2.4</t>
@@ -4019,13 +4019,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="51102087"/>
-        <c:axId val="10914346"/>
+        <c:axId val="14882486"/>
+        <c:axId val="36329381"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="51102087"/>
+        <c:axId val="14882486"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -4063,7 +4063,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10914346"/>
+        <c:crossAx val="36329381"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4071,7 +4071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10914346"/>
+        <c:axId val="36329381"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4114,7 +4114,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51102087"/>
+        <c:crossAx val="14882486"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4178,9 +4178,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>14760</xdr:colOff>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4189,7 +4189,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="13680" y="4572720"/>
-        <a:ext cx="10967040" cy="9331560"/>
+        <a:ext cx="10966680" cy="9331200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -7598,7 +7598,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7969,7 +7969,7 @@
       <c r="I15" s="17"/>
       <c r="J15" s="21"/>
     </row>
-    <row r="16" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="25.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="44"/>
       <c r="B16" s="106" t="s">
         <v>687</v>
@@ -7984,7 +7984,7 @@
       <c r="F16" s="83" t="s">
         <v>688</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="24" t="s">
         <v>13</v>
       </c>
       <c r="H16" s="24"/>
@@ -8022,7 +8022,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10019,7 +10019,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -12554,8 +12554,8 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>